<commit_message>
Adds some info about sessions.
</commit_message>
<xml_diff>
--- a/data/RSE Workshop Applications V2 RS.xlsx
+++ b/data/RSE Workshop Applications V2 RS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livewarwickac.sharepoint.com/sites/dataaiworkshop/Shared Documents/Programme/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B90CC8B9-2D0B-4757-B31A-41381A094E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{13AC82AF-073F-47A4-B52C-665413D25FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,11 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Applications!$A$1:$X$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Schedule_v2!$A$1:$L$43</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="10299" r:id="rId5"/>
+    <pivotCache cacheId="10695" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="488">
   <si>
     <t>ID</t>
   </si>
@@ -1258,6 +1259,9 @@
     <t>Lunch</t>
   </si>
   <si>
+    <t>Meal will be served. Enjoy the food and the company!</t>
+  </si>
+  <si>
     <t>13:30-13:45</t>
   </si>
   <si>
@@ -1292,6 +1296,9 @@
   </si>
   <si>
     <t>Break  &amp; Poster Session 1</t>
+  </si>
+  <si>
+    <t>Some minutes for relaxing and networking. Poster's authors will be presenting their work.</t>
   </si>
   <si>
     <t>16:30-16:00</t>
@@ -1332,6 +1339,9 @@
   </si>
   <si>
     <t>Break</t>
+  </si>
+  <si>
+    <t>Some minutes for relaxing and networking</t>
   </si>
   <si>
     <t>19:00-20:00</t>
@@ -3323,7 +3333,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{92A790C9-6434-48BC-84C6-38AF212FD902}" name="Taula dinàmica1" cacheId="10299" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valors" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{92A790C9-6434-48BC-84C6-38AF212FD902}" name="Taula dinàmica1" cacheId="10695" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valors" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A2:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="23">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -6295,8 +6305,8 @@
   <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I40" sqref="I40"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -6364,28 +6374,31 @@
       <c r="C2" s="7" t="s">
         <v>377</v>
       </c>
+      <c r="J2" s="7" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="7" t="s">
         <v>375</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1">
@@ -6393,22 +6406,22 @@
         <v>375</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>65</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1">
@@ -6416,10 +6429,13 @@
         <v>375</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>389</v>
+        <v>390</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1">
@@ -6427,16 +6443,16 @@
         <v>375</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F6">
         <v>568593183</v>
@@ -6454,7 +6470,7 @@
         <v>68</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1">
@@ -6462,16 +6478,16 @@
         <v>375</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="F7" s="7">
         <v>569241216</v>
@@ -6483,10 +6499,10 @@
         <v>190</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1">
@@ -6494,16 +6510,16 @@
         <v>375</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="F8" s="7">
         <v>569356062</v>
@@ -6515,10 +6531,10 @@
         <v>211</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1">
@@ -6526,10 +6542,13 @@
         <v>375</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>402</v>
+        <v>404</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1">
@@ -6537,24 +6556,27 @@
         <v>375</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>404</v>
+        <v>407</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>167</v>
@@ -6577,16 +6599,16 @@
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>167</v>
@@ -6601,24 +6623,24 @@
         <v>273</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>167</v>
@@ -6633,35 +6655,38 @@
         <v>160</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1">
       <c r="A14" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="J14" s="7" t="s">
         <v>405</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>414</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1">
       <c r="A15" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>228</v>
@@ -6684,16 +6709,16 @@
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>228</v>
@@ -6716,16 +6741,16 @@
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1">
       <c r="A17" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>228</v>
@@ -6740,15 +6765,15 @@
         <v>241</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1">
       <c r="A18" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>376</v>
@@ -6756,22 +6781,25 @@
       <c r="C18" s="7" t="s">
         <v>377</v>
       </c>
+      <c r="J18" s="7" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1">
       <c r="A19" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="F19">
         <v>569324797</v>
@@ -6791,19 +6819,19 @@
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1">
       <c r="A20" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="F20">
         <v>569371846</v>
@@ -6823,19 +6851,19 @@
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1">
       <c r="A21" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>422</v>
-      </c>
       <c r="D21" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="F21">
         <v>569366214</v>
@@ -6847,40 +6875,42 @@
         <v>266</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22"/>
       <c r="G22"/>
       <c r="H22"/>
-      <c r="J22" s="10"/>
+      <c r="J22" s="7" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1">
       <c r="A23" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E23" t="s">
         <v>156</v>
@@ -6903,16 +6933,16 @@
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1">
       <c r="A24" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>156</v>
@@ -6927,24 +6957,24 @@
         <v>181</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1">
       <c r="A25" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>156</v>
@@ -6959,58 +6989,62 @@
         <v>292</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1">
       <c r="A26" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26"/>
       <c r="G26"/>
       <c r="H26"/>
-      <c r="J26" s="10"/>
+      <c r="J26" s="7" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="27" spans="1:10" ht="15" customHeight="1">
       <c r="A27" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27"/>
       <c r="G27"/>
       <c r="H27"/>
-      <c r="J27" s="10"/>
+      <c r="J27" s="7" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1">
       <c r="A28" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28">
@@ -7023,7 +7057,7 @@
         <v>90</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="J28" s="10" t="s">
         <v>284</v>
@@ -7031,16 +7065,16 @@
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1">
       <c r="A29" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29">
@@ -7053,24 +7087,24 @@
         <v>292</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1">
       <c r="A30" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30">
@@ -7091,16 +7125,16 @@
     </row>
     <row r="31" spans="1:10" ht="15" customHeight="1">
       <c r="A31" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31">
@@ -7121,16 +7155,16 @@
     </row>
     <row r="32" spans="1:10" ht="15" customHeight="1">
       <c r="A32" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32">
@@ -7151,16 +7185,16 @@
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1">
       <c r="A33" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B33" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>444</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>441</v>
-      </c>
       <c r="D33" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E33" s="9"/>
       <c r="F33">
@@ -7181,16 +7215,16 @@
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1">
       <c r="A34" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E34" s="9"/>
       <c r="F34">
@@ -7211,16 +7245,16 @@
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1">
       <c r="A35" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35">
@@ -7233,74 +7267,76 @@
         <v>84</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1">
       <c r="A36" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="F36"/>
       <c r="G36"/>
       <c r="H36"/>
-      <c r="J36" s="10"/>
+      <c r="J36" s="7" t="s">
+        <v>391</v>
+      </c>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1">
       <c r="A37" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E37" s="9"/>
       <c r="G37" s="7" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="I37" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1">
       <c r="A38" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="E38" s="9"/>
       <c r="G38" s="10" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" customHeight="1">
       <c r="A39" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>376</v>
@@ -7313,20 +7349,22 @@
       <c r="F39"/>
       <c r="G39"/>
       <c r="H39"/>
-      <c r="J39" s="10"/>
+      <c r="J39" s="7" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1">
       <c r="A40" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>133</v>
@@ -7341,7 +7379,7 @@
         <v>108</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="J40" s="7" t="s">
         <v>129</v>
@@ -7349,16 +7387,16 @@
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1">
       <c r="A41" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E41" s="9" t="s">
         <v>133</v>
@@ -7381,23 +7419,23 @@
     </row>
     <row r="42" spans="1:10" ht="15" customHeight="1">
       <c r="A42" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E42" s="9"/>
       <c r="G42" s="7" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" customHeight="1">
@@ -7405,10 +7443,10 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E43" s="9"/>
       <c r="F43"/>
@@ -7524,6 +7562,7 @@
       <c r="E87" s="9"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L43" xr:uid="{B6FC7663-D29B-47D4-8AE2-312759209D09}"/>
   <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7602,10 +7641,10 @@
         <v>375</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
@@ -7613,19 +7652,19 @@
         <v>375</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
@@ -7633,7 +7672,7 @@
         <v>375</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1">
@@ -7641,10 +7680,10 @@
         <v>375</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>133</v>
@@ -7670,10 +7709,10 @@
         <v>375</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>133</v>
@@ -7699,10 +7738,10 @@
         <v>375</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>133</v>
@@ -7723,7 +7762,7 @@
         <v>68</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
@@ -7731,13 +7770,13 @@
         <v>375</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E9" s="7">
         <v>569241216</v>
@@ -7749,10 +7788,10 @@
         <v>190</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
@@ -7760,13 +7799,13 @@
         <v>375</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E10" s="7">
         <v>569356062</v>
@@ -7778,10 +7817,10 @@
         <v>211</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1">
@@ -7789,17 +7828,17 @@
         <v>375</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="7" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
@@ -7807,10 +7846,10 @@
         <v>375</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1">
@@ -7818,21 +7857,21 @@
         <v>375</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>167</v>
@@ -7855,13 +7894,13 @@
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
       <c r="A15" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>167</v>
@@ -7876,21 +7915,21 @@
         <v>273</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>167</v>
@@ -7905,21 +7944,21 @@
         <v>160</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1">
       <c r="A17" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>228</v>
@@ -7942,13 +7981,13 @@
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1">
       <c r="A18" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>228</v>
@@ -7971,13 +8010,13 @@
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1">
       <c r="A19" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>228</v>
@@ -7992,37 +8031,37 @@
         <v>241</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1">
       <c r="A20" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1">
       <c r="A21" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="D21" s="9"/>
       <c r="F21" s="7" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>131</v>
@@ -8030,43 +8069,43 @@
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1">
       <c r="A23" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>479</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>476</v>
       </c>
       <c r="D23" s="9"/>
       <c r="F23" s="10" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1">
       <c r="A24" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24">
@@ -8079,7 +8118,7 @@
         <v>90</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>284</v>
@@ -8087,28 +8126,28 @@
     </row>
     <row r="25" spans="1:9" ht="15" customHeight="1">
       <c r="A25" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1">
       <c r="A26" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="E26">
         <v>569324797</v>
@@ -8128,16 +8167,16 @@
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1">
       <c r="A27" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="E27">
         <v>569371846</v>
@@ -8157,16 +8196,16 @@
     </row>
     <row r="28" spans="1:9" ht="15" customHeight="1">
       <c r="A28" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="E28">
         <v>569366214</v>
@@ -8178,21 +8217,21 @@
         <v>266</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1">
       <c r="A29" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="D29" t="s">
         <v>156</v>
@@ -8215,13 +8254,13 @@
     </row>
     <row r="30" spans="1:9" ht="15" customHeight="1">
       <c r="A30" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>156</v>
@@ -8236,21 +8275,21 @@
         <v>181</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15" customHeight="1">
       <c r="A31" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>156</v>
@@ -8265,45 +8304,45 @@
         <v>292</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1">
       <c r="A32" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="D32" s="9"/>
     </row>
     <row r="33" spans="1:9" ht="15" customHeight="1">
       <c r="A33" s="7" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="D33" s="9"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1">
       <c r="A34" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34">
@@ -8316,21 +8355,21 @@
         <v>292</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" customHeight="1">
       <c r="A35" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35">
@@ -8351,13 +8390,13 @@
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1">
       <c r="A36" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36">
@@ -8378,13 +8417,13 @@
     </row>
     <row r="37" spans="1:9" ht="15" customHeight="1">
       <c r="A37" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37">
@@ -8405,13 +8444,13 @@
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1">
       <c r="A38" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B38" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>444</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>441</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38">
@@ -8432,13 +8471,13 @@
     </row>
     <row r="39" spans="1:9" ht="15" customHeight="1">
       <c r="A39" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39">
@@ -8459,13 +8498,13 @@
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1">
       <c r="A40" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40">
@@ -8478,51 +8517,51 @@
         <v>84</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15" customHeight="1">
       <c r="A41" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1">
       <c r="A42" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D42" s="9"/>
       <c r="F42" s="7" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15" customHeight="1">
       <c r="A43" s="7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="D43" s="9"/>
     </row>
@@ -8553,7 +8592,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -8654,12 +8693,12 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="B16">
         <v>29</v>
@@ -8671,12 +8710,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="6d669ffc-f96f-45b1-8cef-205faefb68e0">
+      <UserInfo>
+        <DisplayName>Silver, Rebecca</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Barnes, Casey</DisplayName>
+        <AccountId>23</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Turner, Heather</DisplayName>
+        <AccountId>11</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8845,31 +8899,16 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="6d669ffc-f96f-45b1-8cef-205faefb68e0">
-      <UserInfo>
-        <DisplayName>Silver, Rebecca</DisplayName>
-        <AccountId>13</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Barnes, Casey</DisplayName>
-        <AccountId>23</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Turner, Heather</DisplayName>
-        <AccountId>11</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AD4B4FE-F1B3-4850-A8E8-D27F8EC6450F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D96BB6B0-67E0-417D-88A6-CD80AF7E5A4A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8877,5 +8916,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D96BB6B0-67E0-417D-88A6-CD80AF7E5A4A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AD4B4FE-F1B3-4850-A8E8-D27F8EC6450F}"/>
 </file>
</xml_diff>

<commit_message>
Regenerate schedule with updated changes
</commit_message>
<xml_diff>
--- a/data/RSE Workshop Applications V2 RS.xlsx
+++ b/data/RSE Workshop Applications V2 RS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livewarwickac.sharepoint.com/sites/dataaiworkshop/Shared Documents/Programme/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13AC82AF-073F-47A4-B52C-665413D25FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B49E0829-1608-4F4E-A6BB-45208FCEFAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="10695" r:id="rId5"/>
+    <pivotCache cacheId="13216" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="487">
   <si>
     <t>ID</t>
   </si>
@@ -1289,7 +1289,13 @@
     <t>Martin O’Reilly</t>
   </si>
   <si>
-    <t>The Data Safe Haven</t>
+    <t>The Data Safe Haven: An open, scalable, reproducibly deployable, cloud-based Trusted Research Environment for working safely with sensitive data</t>
+  </si>
+  <si>
+    <t>Researchers often need to analyse sensitive data in order to answer important questions for health, government and society. Balancing the need to protect individual privacy and commercial confidentiality with the need to ensure that reliable insights can be made using sensitive data is challenging, and Trusted Research Environments (TREs) that provide secure analysis environments for working  with sensitive data are a key part of striking this balance.
+The Alan Turing Institute has recently open-sourced its Data Safe Haven, a secure, scalable, reproducibly deployable, cloud-based TRE that we have been using for the lat 4 years to support our researchers in working safely and productively with sensitive data. By openly publishing the code and documentation required to deploy, configure and manage a Data Safe Haven instance, we make it easier for others to deploy their own Trusted Research Environments, reducing the effort required to support their researchers in working safely with sensitive data.
+We've also been working closely with the wider community to better align work in this area, initially on the development of the information governance principals and design choices for our Data Safe Haven, which we published in 2019. More recently, we've been working closely with the DARE UK programme to define common requirements for Trusted Research Environments and have co-founded the RSE TRE Community, bringing together those who are developing and deploying TREs to more closely co-ordinate our work.
+In this talk we will give an overview of the Turing's Data Safe Haven and the information governance and design principals behind it, as well as the work we have been doing with the wider community to develop a common set of TRE requirements and to co-ordinate across organisations on the development, deployment and management of TREs.</t>
   </si>
   <si>
     <t>14:45-15:30</t>
@@ -1314,9 +1320,6 @@
   </si>
   <si>
     <t>16:00-16:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supporting medical research and practice </t>
   </si>
   <si>
     <t>Statisticians embarking into the realm of Research Software Engineering</t>
@@ -1538,16 +1541,10 @@
     <t>Intro</t>
   </si>
   <si>
-    <t>The Data Safe Haven: An open, scalable, reproducibly deployable, cloud-based Trusted Research Environment for working safely with sensitive data</t>
-  </si>
-  <si>
-    <t>Researchers often need to analyse sensitive data in order to answer important questions for health, government and society. Balancing the need to protect individual privacy and commercial confidentiality with the need to ensure that reliable insights can be made using sensitive data is challenging, and Trusted Research Environments (TREs) that provide secure analysis environments for working  with sensitive data are a key part of striking this balance.
-The Alan Turing Institute has recently open-sourced its Data Safe Haven, a secure, scalable, reproducibly deployable, cloud-based TRE that we have been using for the lat 4 years to support our researchers in working safely and productively with sensitive data. By openly publishing the code and documentation required to deploy, configure and manage a Data Safe Haven instance, we make it easier for others to deploy their own Trusted Research Environments, reducing the effort required to support their researchers in working safely with sensitive data.
-We've also been working closely with the wider community to better align work in this area, initially on the development of the information governance principals and design choices for our Data Safe Haven, which we published in 2019. More recently, we've been working closely with the DARE UK programme to define common requirements for Trusted Research Environments and have co-founded the RSE TRE Community, bringing together those who are developing and deploying TREs to more closely co-ordinate our work.
-In this talk we will give an overview of the Turing's Data Safe Haven and the information governance and design principals behind it, as well as the work we have been doing with the wider community to develop a common set of TRE requirements and to co-ordinate across organisations on the development, deployment and management of TREs.</t>
-  </si>
-  <si>
     <t>17:00-17:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supporting medical research and practice </t>
   </si>
   <si>
     <t>3rd talk  ID 568876112 dropped out</t>
@@ -3333,7 +3330,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{92A790C9-6434-48BC-84C6-38AF212FD902}" name="Taula dinàmica1" cacheId="10695" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valors" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{92A790C9-6434-48BC-84C6-38AF212FD902}" name="Taula dinàmica1" cacheId="13216" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valors" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A2:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="23">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -6305,8 +6302,8 @@
   <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -6420,8 +6417,11 @@
       <c r="H4" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="13" t="s">
         <v>388</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1">
@@ -6429,13 +6429,13 @@
         <v>375</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1">
@@ -6443,16 +6443,16 @@
         <v>375</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>381</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="F6">
         <v>568593183</v>
@@ -6470,7 +6470,7 @@
         <v>68</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1">
@@ -6478,16 +6478,16 @@
         <v>375</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>381</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>397</v>
+      <c r="E7" s="14" t="s">
+        <v>395</v>
       </c>
       <c r="F7" s="7">
         <v>569241216</v>
@@ -6513,13 +6513,13 @@
         <v>400</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>381</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>397</v>
+      <c r="E8" s="14" t="s">
+        <v>395</v>
       </c>
       <c r="F8" s="7">
         <v>569356062</v>
@@ -6936,7 +6936,7 @@
         <v>408</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>433</v>
@@ -7289,7 +7289,7 @@
       <c r="G36"/>
       <c r="H36"/>
       <c r="J36" s="7" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1">
@@ -7573,8 +7573,8 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <pane ySplit="1" topLeftCell="H2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -7661,10 +7661,10 @@
         <v>387</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>468</v>
+        <v>388</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>469</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
@@ -7680,10 +7680,10 @@
         <v>375</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>133</v>
@@ -7712,7 +7712,7 @@
         <v>400</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>133</v>
@@ -7738,10 +7738,10 @@
         <v>375</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>133</v>
@@ -7762,7 +7762,7 @@
         <v>68</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
@@ -7770,13 +7770,13 @@
         <v>375</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>397</v>
+        <v>469</v>
       </c>
       <c r="E9" s="7">
         <v>569241216</v>
@@ -7802,10 +7802,10 @@
         <v>400</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>397</v>
+        <v>469</v>
       </c>
       <c r="E10" s="7">
         <v>569356062</v>
@@ -7828,17 +7828,17 @@
         <v>375</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>397</v>
+        <v>469</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
@@ -7846,7 +7846,7 @@
         <v>375</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>404</v>
@@ -7857,10 +7857,10 @@
         <v>375</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>473</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1">
@@ -7868,7 +7868,7 @@
         <v>408</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>410</v>
@@ -7897,7 +7897,7 @@
         <v>408</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>410</v>
@@ -7955,7 +7955,7 @@
         <v>408</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>410</v>
@@ -7984,7 +7984,7 @@
         <v>408</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>410</v>
@@ -8045,7 +8045,7 @@
         <v>417</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D20" s="9"/>
     </row>
@@ -8054,10 +8054,10 @@
         <v>408</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>478</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>479</v>
       </c>
       <c r="D21" s="9"/>
       <c r="F21" s="7" t="s">
@@ -8072,10 +8072,10 @@
         <v>408</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>480</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>481</v>
       </c>
       <c r="D22" s="9"/>
     </row>
@@ -8084,10 +8084,10 @@
         <v>408</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D23" s="9"/>
       <c r="F23" s="10" t="s">
@@ -8105,7 +8105,7 @@
         <v>431</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24">
@@ -8132,7 +8132,7 @@
         <v>432</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D25" s="9"/>
     </row>
@@ -8141,7 +8141,7 @@
         <v>408</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>419</v>
@@ -8199,7 +8199,7 @@
         <v>408</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>419</v>
@@ -8228,7 +8228,7 @@
         <v>408</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>419</v>
@@ -8286,7 +8286,7 @@
         <v>408</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>419</v>
@@ -8315,10 +8315,10 @@
         <v>408</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D32" s="9"/>
     </row>
@@ -8327,10 +8327,10 @@
         <v>408</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D33" s="9"/>
     </row>
@@ -8342,7 +8342,7 @@
         <v>409</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34">
@@ -8531,7 +8531,7 @@
         <v>417</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D41" s="9"/>
     </row>
@@ -8540,7 +8540,7 @@
         <v>438</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>386</v>
@@ -8558,10 +8558,10 @@
         <v>438</v>
       </c>
       <c r="B43" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>480</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>481</v>
       </c>
       <c r="D43" s="9"/>
     </row>
@@ -8592,7 +8592,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -8693,12 +8693,12 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B16">
         <v>29</v>
@@ -8710,30 +8710,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="6d669ffc-f96f-45b1-8cef-205faefb68e0">
-      <UserInfo>
-        <DisplayName>Silver, Rebecca</DisplayName>
-        <AccountId>13</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Barnes, Casey</DisplayName>
-        <AccountId>23</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Turner, Heather</DisplayName>
-        <AccountId>11</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010030B0E3D86AF8E94EB0D779FA2A578701" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a43da20c1e4d4a0fa4cb6e9a264adb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5c1e5410-6003-4dcc-aaff-e929c276a0f6" xmlns:ns3="6d669ffc-f96f-45b1-8cef-205faefb68e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a33243bcbacded30e9c35f3ebd27a0f3" ns2:_="" ns3:_="">
     <xsd:import namespace="5c1e5410-6003-4dcc-aaff-e929c276a0f6"/>
@@ -8898,7 +8874,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -8907,14 +8883,38 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="6d669ffc-f96f-45b1-8cef-205faefb68e0">
+      <UserInfo>
+        <DisplayName>Silver, Rebecca</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Barnes, Casey</DisplayName>
+        <AccountId>23</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Turner, Heather</DisplayName>
+        <AccountId>11</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D96BB6B0-67E0-417D-88A6-CD80AF7E5A4A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEBADE79-20BE-441D-93C8-2DC337480A5F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEBADE79-20BE-441D-93C8-2DC337480A5F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AD4B4FE-F1B3-4850-A8E8-D27F8EC6450F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AD4B4FE-F1B3-4850-A8E8-D27F8EC6450F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D96BB6B0-67E0-417D-88A6-CD80AF7E5A4A}"/>
 </file>
</xml_diff>